<commit_message>
Update a test boss
</commit_message>
<xml_diff>
--- a/Assets/Datas/DialogData.xlsx
+++ b/Assets/Datas/DialogData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>DialogID</t>
   </si>
@@ -49,6 +49,15 @@
     <t>空格键：跳跃
 鼠标左键：攻击
 左SHIFT：冲刺</t>
+  </si>
+  <si>
+    <t>您好，南京大学的招生老师！</t>
+  </si>
+  <si>
+    <t>感谢您观看我的视频！</t>
+  </si>
+  <si>
+    <t>这是让不懂编程的人做剧本用的。</t>
   </si>
 </sst>
 </file>
@@ -890,20 +899,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -969,6 +977,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>